<commit_message>
Proceso mostrado y validado en UAT
</commit_message>
<xml_diff>
--- a/Data/Summary/Report.xlsx
+++ b/Data/Summary/Report.xlsx
@@ -34,28 +34,70 @@
     <x:t>1</x:t>
   </x:si>
   <x:si>
-    <x:t>00837202408281501154-29082024</x:t>
+    <x:t>00837202409271520249-01102024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BE</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Error BusinessRule process state: No se han encontrado casos pendientes de procesar</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TransactionTime: 0h 2m 2s</x:t>
+  </x:si>
+  <x:si>
+    <x:t>2</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00837202409271514903-01102024</x:t>
   </x:si>
   <x:si>
     <x:t>OK</x:t>
   </x:si>
   <x:si>
-    <x:t>Successful Transaction: 1 - Reference: 00837202408281501154-29082024</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TransactionTime: 0h 0m 27s</x:t>
-  </x:si>
-  <x:si>
-    <x:t>2</x:t>
-  </x:si>
-  <x:si>
-    <x:t>00837202408271500357-29082024</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Successful Transaction: 2 - Reference: 00837202408271500357-29082024</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TransactionTime: 0h 0m 26s</x:t>
+    <x:t>Successful Transaction: 2 - Reference: 00837202409271514903-01102024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TransactionTime: 0h 0m 34s</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00837202409271514879-01102024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TransactionTime: 0h 1m 23s</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00837202409271514149-01102024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TransactionTime: 0h 1m 0s</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00837202409271513999-01102024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TransactionTime: 0h 0m 59s</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>00837202409161511213-18092024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Error BusinessRule process state: No se encontrarón datos en detalle del item: 00837202409161511213</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TransactionTime: 0h 0m 42s</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -454,13 +496,81 @@
         <x:v>11</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:5">
+      <x:c r="A4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s">
-        <x:v>12</x:v>
-      </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>13</x:v>
+      <x:c r="D4" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:5">
+      <x:c r="A5" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="C5" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="6" spans="1:5">
+      <x:c r="A6" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>23</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:5">
+      <x:c r="A7" s="0" t="s">
+        <x:v>24</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>25</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>7</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>27</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>

<commit_message>
Se ajuste foco aplicación InfoNova a traves del selector
</commit_message>
<xml_diff>
--- a/Data/Summary/Report.xlsx
+++ b/Data/Summary/Report.xlsx
@@ -38,19 +38,25 @@
     <x:t>TiempoTransaccion</x:t>
   </x:si>
   <x:si>
+    <x:t>Rango Final</x:t>
+  </x:si>
+  <x:si>
     <x:t>1</x:t>
   </x:si>
   <x:si>
-    <x:t>00837202410011519083-04102024</x:t>
-  </x:si>
-  <x:si>
-    <x:t>BE</x:t>
-  </x:si>
-  <x:si>
-    <x:t>Error BusinessRule process state: No se han encontrado casos pendientes de procesar</x:t>
-  </x:si>
-  <x:si>
-    <x:t>TransactionTime: 0h 0m 36s</x:t>
+    <x:t>00837202410161513058-18102024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>OK</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Successful Transaction: 1 - Reference: 00837202410161513058-18102024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>TransactionTime: 0h 1m 36s</x:t>
+  </x:si>
+  <x:si>
+    <x:t>948690199</x:t>
   </x:si>
   <x:si>
     <x:t>2</x:t>
@@ -79,6 +85,9 @@
   </x:si>
   <x:si>
     <x:t>00837202410011513601-04102024</x:t>
+  </x:si>
+  <x:si>
+    <x:t>BE</x:t>
   </x:si>
   <x:si>
     <x:t>Error BusinessRule process state: No se ha encontrado ningún caso de la categoria: 'Operaciones de aprovisionamiento Voip Port-in'</x:t>
@@ -446,7 +455,7 @@
   </x:sheetViews>
   <x:sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <x:sheetData>
-    <x:row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <x:row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -462,73 +471,79 @@
       <x:c r="E1" s="0" t="s">
         <x:v>4</x:v>
       </x:c>
+      <x:c r="F1" s="0" t="s">
+        <x:v>5</x:v>
+      </x:c>
     </x:row>
-    <x:row r="2" spans="1:5">
+    <x:row r="2" spans="1:6">
       <x:c r="A2" s="0" t="s">
-        <x:v>5</x:v>
+        <x:v>6</x:v>
       </x:c>
       <x:c r="B2" s="0" t="s">
-        <x:v>6</x:v>
+        <x:v>7</x:v>
       </x:c>
       <x:c r="C2" s="0" t="s">
-        <x:v>7</x:v>
+        <x:v>8</x:v>
       </x:c>
       <x:c r="D2" s="0" t="s">
-        <x:v>8</x:v>
+        <x:v>9</x:v>
       </x:c>
       <x:c r="E2" s="0" t="s">
-        <x:v>9</x:v>
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="F2" s="0" t="s">
+        <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:5">
+    <x:row r="3" spans="1:6">
       <x:c r="A3" s="0" t="s">
-        <x:v>10</x:v>
+        <x:v>12</x:v>
       </x:c>
       <x:c r="B3" s="0" t="s">
-        <x:v>11</x:v>
+        <x:v>13</x:v>
       </x:c>
       <x:c r="C3" s="0" t="s">
-        <x:v>12</x:v>
+        <x:v>14</x:v>
       </x:c>
       <x:c r="D3" s="1" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:6">
+      <x:c r="A4" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="B4" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="C4" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>20</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>21</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:6">
+      <x:c r="A5" s="0" t="s">
+        <x:v>22</x:v>
+      </x:c>
+      <x:c r="B5" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="E3" s="0" t="s">
-        <x:v>14</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="4" spans="1:5">
-      <x:c r="A4" s="0" t="s">
-        <x:v>15</x:v>
-      </x:c>
-      <x:c r="B4" s="0" t="s">
-        <x:v>16</x:v>
-      </x:c>
-      <x:c r="C4" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
-      <x:c r="D4" s="0" t="s">
-        <x:v>17</x:v>
-      </x:c>
-      <x:c r="E4" s="0" t="s">
-        <x:v>18</x:v>
-      </x:c>
-    </x:row>
-    <x:row r="5" spans="1:5">
-      <x:c r="A5" s="0" t="s">
+      <x:c r="C5" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="B5" s="0" t="s">
-        <x:v>11</x:v>
-      </x:c>
-      <x:c r="C5" s="0" t="s">
-        <x:v>7</x:v>
-      </x:c>
       <x:c r="D5" s="0" t="s">
-        <x:v>17</x:v>
+        <x:v>20</x:v>
       </x:c>
       <x:c r="E5" s="0" t="s">
-        <x:v>20</x:v>
+        <x:v>23</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>